<commit_message>
Embedded image in excel template is not printed on each band row 928
</commit_message>
<xml_diff>
--- a/jmix-reports/reports/src/test/resources/xlsx/template.xlsx
+++ b/jmix-reports/reports/src/test/resources/xlsx/template.xlsx
@@ -8,11 +8,13 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="headerUsers" vbProcedure="false">Sheet1!$A$2:$B$2</definedName>
     <definedName function="false" hidden="false" name="Users" vbProcedure="false">Sheet1!$A$3:$B$3</definedName>
+    <definedName function="false" hidden="false" name="Users2" vbProcedure="false">Sheet2!$A$2:$B$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -163,9 +165,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1071720</xdr:colOff>
+      <xdr:colOff>1070280</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>799920</xdr:rowOff>
+      <xdr:rowOff>798480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -178,8 +180,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2669760" y="511560"/>
-          <a:ext cx="687960" cy="669240"/>
+          <a:off x="2673720" y="1018440"/>
+          <a:ext cx="686520" cy="667800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -200,9 +202,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2012760</xdr:colOff>
+      <xdr:colOff>2011320</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>826560</xdr:rowOff>
+      <xdr:rowOff>825120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -215,8 +217,45 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3580560" y="489240"/>
-          <a:ext cx="718200" cy="718200"/>
+          <a:off x="3584520" y="996120"/>
+          <a:ext cx="716760" cy="716760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>421560</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>156240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1688040</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>555840</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 4" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="421560" y="156240"/>
+          <a:ext cx="1266480" cy="399600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -231,129 +270,65 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1819440</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>10080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2505960</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>677880</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 3" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4132800" y="172800"/>
+          <a:ext cx="686520" cy="667800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
         </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.51953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="30"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1" customFormat="false" ht="54.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>0</v>
@@ -380,4 +355,41 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.22"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="67.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>